<commit_message>
Alterações de logica pt2
</commit_message>
<xml_diff>
--- a/Compras.xlsx
+++ b/Compras.xlsx
@@ -656,7 +656,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CAM VERM POLO</t>
+          <t xml:space="preserve">CAM VERM POLO </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1941,7 +1941,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E6" t="n">
         <v>31</v>

</xml_diff>

<commit_message>
Limpeza automatica de caixa
</commit_message>
<xml_diff>
--- a/Compras.xlsx
+++ b/Compras.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="4020" windowWidth="20460" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Caixa" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,12 +18,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -41,9 +40,6 @@
       <b val="1"/>
       <sz val="11"/>
     </font>
-    <font>
-      <b val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -53,7 +49,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -121,17 +117,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -147,9 +137,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -519,465 +506,74 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="16.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="9" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="9" customWidth="1" min="4" max="4"/>
-    <col width="8.7109375" customWidth="1" min="5" max="5"/>
-    <col width="19.5703125" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="19.5703125" customWidth="1" min="9" max="9"/>
-    <col width="14.140625" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" min="12" max="12"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Operação</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Tamanho</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Sexo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Desconto</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Forma Pag</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Valor unitario compra</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Valor unitario venda</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Valor recebido</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Valor a receber</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Compra</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Compra A</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>A vista</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I2" t="n">
-        <v>50</v>
-      </c>
-      <c r="J2" t="n">
-        <v>50</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>46047.375</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Compra</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Compra B</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>A vista</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>31</v>
-      </c>
-      <c r="I3" t="n">
-        <v>50</v>
-      </c>
-      <c r="J3" t="n">
-        <v>50</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2" t="n">
-        <v>46047.41666666666</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Venda A</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>36</v>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>A vista</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>31</v>
-      </c>
-      <c r="I4" t="n">
-        <v>50</v>
-      </c>
-      <c r="J4" t="n">
-        <v>50</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2" t="n">
-        <v>46047.45833333334</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Venda B</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>37</v>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>A vista</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>31</v>
-      </c>
-      <c r="I5" t="n">
-        <v>50</v>
-      </c>
-      <c r="J5" t="n">
-        <v>50</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2" t="n">
-        <v>46047.5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Compra</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CAM VERM POLO </t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>GG</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>A vista</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>31</v>
-      </c>
-      <c r="I6" t="n">
-        <v>50</v>
-      </c>
-      <c r="J6" t="n">
-        <v>50</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2" t="n">
-        <v>46047.54166666666</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CAM VERM POLO </t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>GG</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>A vista</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>31</v>
-      </c>
-      <c r="I7" t="n">
-        <v>50</v>
-      </c>
-      <c r="J7" t="n">
-        <v>50</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2" t="n">
-        <v>46047.58333333334</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Venda</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CAM VERM POLO </t>
-        </is>
-      </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>GG</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>A vista</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>31</v>
-      </c>
-      <c r="I8" t="n">
-        <v>50</v>
-      </c>
-      <c r="J8" t="n">
-        <v>50</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2" t="n">
-        <v>46047.54166666666</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Compra</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CAM VERM POLO </t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="inlineStr">
-        <is>
-          <t>GG</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>100</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>A vista</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>31</v>
-      </c>
-      <c r="I9" t="n">
-        <v>50</v>
-      </c>
-      <c r="J9" t="n">
-        <v>50</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2" t="n">
-        <v>45682.54166666666</v>
       </c>
     </row>
   </sheetData>
@@ -991,7 +587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F273"/>
+  <dimension ref="A1:F285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1000,32 +596,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Tamanho</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Sexo</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Valor unitario compra</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Data da compra</t>
         </is>
@@ -1053,7 +649,7 @@
       <c r="E2" t="n">
         <v>30</v>
       </c>
-      <c r="F2" s="9" t="n">
+      <c r="F2" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1079,7 +675,7 @@
       <c r="E3" t="n">
         <v>30</v>
       </c>
-      <c r="F3" s="9" t="n">
+      <c r="F3" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1105,7 +701,7 @@
       <c r="E4" t="n">
         <v>30</v>
       </c>
-      <c r="F4" s="9" t="n">
+      <c r="F4" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1131,7 +727,7 @@
       <c r="E5" t="n">
         <v>30</v>
       </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1157,7 +753,7 @@
       <c r="E6" t="n">
         <v>30</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1183,7 +779,7 @@
       <c r="E7" t="n">
         <v>30</v>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1209,7 +805,7 @@
       <c r="E8" t="n">
         <v>30</v>
       </c>
-      <c r="F8" s="9" t="n">
+      <c r="F8" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1235,7 +831,7 @@
       <c r="E9" t="n">
         <v>30</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1261,7 +857,7 @@
       <c r="E10" t="n">
         <v>30</v>
       </c>
-      <c r="F10" s="9" t="n">
+      <c r="F10" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1287,7 +883,7 @@
       <c r="E11" t="n">
         <v>30</v>
       </c>
-      <c r="F11" s="9" t="n">
+      <c r="F11" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1313,7 +909,7 @@
       <c r="E12" t="n">
         <v>30</v>
       </c>
-      <c r="F12" s="9" t="n">
+      <c r="F12" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1339,7 +935,7 @@
       <c r="E13" t="n">
         <v>30</v>
       </c>
-      <c r="F13" s="9" t="n">
+      <c r="F13" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1365,7 +961,7 @@
       <c r="E14" t="n">
         <v>30</v>
       </c>
-      <c r="F14" s="9" t="n">
+      <c r="F14" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1391,7 +987,7 @@
       <c r="E15" t="n">
         <v>30</v>
       </c>
-      <c r="F15" s="9" t="n">
+      <c r="F15" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1417,7 +1013,7 @@
       <c r="E16" t="n">
         <v>30</v>
       </c>
-      <c r="F16" s="9" t="n">
+      <c r="F16" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1443,7 +1039,7 @@
       <c r="E17" t="n">
         <v>30</v>
       </c>
-      <c r="F17" s="9" t="n">
+      <c r="F17" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1469,7 +1065,7 @@
       <c r="E18" t="n">
         <v>30</v>
       </c>
-      <c r="F18" s="9" t="n">
+      <c r="F18" s="8" t="n">
         <v>46023</v>
       </c>
     </row>
@@ -1484,14 +1080,13 @@
           <t>GG</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
         <v>100</v>
       </c>
       <c r="E19" t="n">
         <v>31</v>
       </c>
-      <c r="F19" s="9" t="n">
+      <c r="F19" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1506,14 +1101,13 @@
           <t>M</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
         <v>1</v>
       </c>
       <c r="E20" t="n">
         <v>30</v>
       </c>
-      <c r="F20" s="9" t="n">
+      <c r="F20" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1528,14 +1122,13 @@
           <t>M</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>1</v>
       </c>
       <c r="E21" t="n">
         <v>31</v>
       </c>
-      <c r="F21" s="9" t="n">
+      <c r="F21" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1550,14 +1143,13 @@
           <t>GG</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
         <v>1</v>
       </c>
       <c r="E22" t="n">
         <v>31</v>
       </c>
-      <c r="F22" s="9" t="n">
+      <c r="F22" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1583,7 +1175,7 @@
       <c r="E23" t="n">
         <v>31</v>
       </c>
-      <c r="F23" s="9" t="n">
+      <c r="F23" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1609,7 +1201,7 @@
       <c r="E24" t="n">
         <v>30</v>
       </c>
-      <c r="F24" s="9" t="n">
+      <c r="F24" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1635,7 +1227,7 @@
       <c r="E25" t="n">
         <v>31</v>
       </c>
-      <c r="F25" s="9" t="n">
+      <c r="F25" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1661,7 +1253,7 @@
       <c r="E26" t="n">
         <v>31</v>
       </c>
-      <c r="F26" s="9" t="n">
+      <c r="F26" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1687,7 +1279,7 @@
       <c r="E27" t="n">
         <v>31</v>
       </c>
-      <c r="F27" s="9" t="n">
+      <c r="F27" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1713,7 +1305,7 @@
       <c r="E28" t="n">
         <v>30</v>
       </c>
-      <c r="F28" s="9" t="n">
+      <c r="F28" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1739,7 +1331,7 @@
       <c r="E29" t="n">
         <v>31</v>
       </c>
-      <c r="F29" s="9" t="n">
+      <c r="F29" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1765,7 +1357,7 @@
       <c r="E30" t="n">
         <v>31</v>
       </c>
-      <c r="F30" s="9" t="n">
+      <c r="F30" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1791,7 +1383,7 @@
       <c r="E31" t="n">
         <v>31</v>
       </c>
-      <c r="F31" s="9" t="n">
+      <c r="F31" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1817,7 +1409,7 @@
       <c r="E32" t="n">
         <v>30</v>
       </c>
-      <c r="F32" s="9" t="n">
+      <c r="F32" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1843,7 +1435,7 @@
       <c r="E33" t="n">
         <v>31</v>
       </c>
-      <c r="F33" s="9" t="n">
+      <c r="F33" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1869,7 +1461,7 @@
       <c r="E34" t="n">
         <v>31</v>
       </c>
-      <c r="F34" s="9" t="n">
+      <c r="F34" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1895,7 +1487,7 @@
       <c r="E35" t="n">
         <v>31</v>
       </c>
-      <c r="F35" s="9" t="n">
+      <c r="F35" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -1921,7 +1513,7 @@
       <c r="E36" t="n">
         <v>30</v>
       </c>
-      <c r="F36" s="9" t="n">
+      <c r="F36" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -1947,7 +1539,7 @@
       <c r="E37" t="n">
         <v>31</v>
       </c>
-      <c r="F37" s="9" t="n">
+      <c r="F37" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -1973,7 +1565,7 @@
       <c r="E38" t="n">
         <v>31</v>
       </c>
-      <c r="F38" s="9" t="n">
+      <c r="F38" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -1999,7 +1591,7 @@
       <c r="E39" t="n">
         <v>31</v>
       </c>
-      <c r="F39" s="9" t="n">
+      <c r="F39" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2025,7 +1617,7 @@
       <c r="E40" t="n">
         <v>30</v>
       </c>
-      <c r="F40" s="9" t="n">
+      <c r="F40" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2051,7 +1643,7 @@
       <c r="E41" t="n">
         <v>31</v>
       </c>
-      <c r="F41" s="9" t="n">
+      <c r="F41" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2077,7 +1669,7 @@
       <c r="E42" t="n">
         <v>31</v>
       </c>
-      <c r="F42" s="9" t="n">
+      <c r="F42" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2103,7 +1695,7 @@
       <c r="E43" t="n">
         <v>31</v>
       </c>
-      <c r="F43" s="9" t="n">
+      <c r="F43" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2129,7 +1721,7 @@
       <c r="E44" t="n">
         <v>30</v>
       </c>
-      <c r="F44" s="9" t="n">
+      <c r="F44" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2155,7 +1747,7 @@
       <c r="E45" t="n">
         <v>31</v>
       </c>
-      <c r="F45" s="9" t="n">
+      <c r="F45" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2181,7 +1773,7 @@
       <c r="E46" t="n">
         <v>31</v>
       </c>
-      <c r="F46" s="9" t="n">
+      <c r="F46" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2207,7 +1799,7 @@
       <c r="E47" t="n">
         <v>31</v>
       </c>
-      <c r="F47" s="9" t="n">
+      <c r="F47" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2233,7 +1825,7 @@
       <c r="E48" t="n">
         <v>30</v>
       </c>
-      <c r="F48" s="9" t="n">
+      <c r="F48" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2259,7 +1851,7 @@
       <c r="E49" t="n">
         <v>31</v>
       </c>
-      <c r="F49" s="9" t="n">
+      <c r="F49" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2285,7 +1877,7 @@
       <c r="E50" t="n">
         <v>31</v>
       </c>
-      <c r="F50" s="9" t="n">
+      <c r="F50" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2311,7 +1903,7 @@
       <c r="E51" t="n">
         <v>31</v>
       </c>
-      <c r="F51" s="9" t="n">
+      <c r="F51" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2337,7 +1929,7 @@
       <c r="E52" t="n">
         <v>30</v>
       </c>
-      <c r="F52" s="9" t="n">
+      <c r="F52" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2363,7 +1955,7 @@
       <c r="E53" t="n">
         <v>31</v>
       </c>
-      <c r="F53" s="9" t="n">
+      <c r="F53" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2389,7 +1981,7 @@
       <c r="E54" t="n">
         <v>31</v>
       </c>
-      <c r="F54" s="9" t="n">
+      <c r="F54" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2415,7 +2007,7 @@
       <c r="E55" t="n">
         <v>31</v>
       </c>
-      <c r="F55" s="9" t="n">
+      <c r="F55" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2441,7 +2033,7 @@
       <c r="E56" t="n">
         <v>31</v>
       </c>
-      <c r="F56" s="9" t="n">
+      <c r="F56" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2467,7 +2059,7 @@
       <c r="E57" t="n">
         <v>30</v>
       </c>
-      <c r="F57" s="9" t="n">
+      <c r="F57" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2493,7 +2085,7 @@
       <c r="E58" t="n">
         <v>31</v>
       </c>
-      <c r="F58" s="9" t="n">
+      <c r="F58" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2519,7 +2111,7 @@
       <c r="E59" t="n">
         <v>31</v>
       </c>
-      <c r="F59" s="9" t="n">
+      <c r="F59" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2545,7 +2137,7 @@
       <c r="E60" t="n">
         <v>31</v>
       </c>
-      <c r="F60" s="9" t="n">
+      <c r="F60" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2571,7 +2163,7 @@
       <c r="E61" t="n">
         <v>30</v>
       </c>
-      <c r="F61" s="9" t="n">
+      <c r="F61" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2597,7 +2189,7 @@
       <c r="E62" t="n">
         <v>31</v>
       </c>
-      <c r="F62" s="9" t="n">
+      <c r="F62" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2623,7 +2215,7 @@
       <c r="E63" t="n">
         <v>31</v>
       </c>
-      <c r="F63" s="9" t="n">
+      <c r="F63" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2649,7 +2241,7 @@
       <c r="E64" t="n">
         <v>31</v>
       </c>
-      <c r="F64" s="9" t="n">
+      <c r="F64" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2675,7 +2267,7 @@
       <c r="E65" t="n">
         <v>30</v>
       </c>
-      <c r="F65" s="9" t="n">
+      <c r="F65" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2701,7 +2293,7 @@
       <c r="E66" t="n">
         <v>31</v>
       </c>
-      <c r="F66" s="9" t="n">
+      <c r="F66" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2727,7 +2319,7 @@
       <c r="E67" t="n">
         <v>31</v>
       </c>
-      <c r="F67" s="9" t="n">
+      <c r="F67" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2753,7 +2345,7 @@
       <c r="E68" t="n">
         <v>31</v>
       </c>
-      <c r="F68" s="9" t="n">
+      <c r="F68" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2779,7 +2371,7 @@
       <c r="E69" t="n">
         <v>30</v>
       </c>
-      <c r="F69" s="9" t="n">
+      <c r="F69" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2805,7 +2397,7 @@
       <c r="E70" t="n">
         <v>31</v>
       </c>
-      <c r="F70" s="9" t="n">
+      <c r="F70" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2831,7 +2423,7 @@
       <c r="E71" t="n">
         <v>31</v>
       </c>
-      <c r="F71" s="9" t="n">
+      <c r="F71" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2857,7 +2449,7 @@
       <c r="E72" t="n">
         <v>31</v>
       </c>
-      <c r="F72" s="9" t="n">
+      <c r="F72" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2883,7 +2475,7 @@
       <c r="E73" t="n">
         <v>30</v>
       </c>
-      <c r="F73" s="9" t="n">
+      <c r="F73" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -2909,7 +2501,7 @@
       <c r="E74" t="n">
         <v>31</v>
       </c>
-      <c r="F74" s="9" t="n">
+      <c r="F74" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -2935,7 +2527,7 @@
       <c r="E75" t="n">
         <v>31</v>
       </c>
-      <c r="F75" s="9" t="n">
+      <c r="F75" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -2961,7 +2553,7 @@
       <c r="E76" t="n">
         <v>31</v>
       </c>
-      <c r="F76" s="9" t="n">
+      <c r="F76" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -2987,7 +2579,7 @@
       <c r="E77" t="n">
         <v>30</v>
       </c>
-      <c r="F77" s="9" t="n">
+      <c r="F77" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3013,7 +2605,7 @@
       <c r="E78" t="n">
         <v>31</v>
       </c>
-      <c r="F78" s="9" t="n">
+      <c r="F78" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3039,7 +2631,7 @@
       <c r="E79" t="n">
         <v>31</v>
       </c>
-      <c r="F79" s="9" t="n">
+      <c r="F79" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3065,7 +2657,7 @@
       <c r="E80" t="n">
         <v>31</v>
       </c>
-      <c r="F80" s="9" t="n">
+      <c r="F80" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3091,7 +2683,7 @@
       <c r="E81" t="n">
         <v>30</v>
       </c>
-      <c r="F81" s="9" t="n">
+      <c r="F81" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3117,7 +2709,7 @@
       <c r="E82" t="n">
         <v>31</v>
       </c>
-      <c r="F82" s="9" t="n">
+      <c r="F82" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3143,7 +2735,7 @@
       <c r="E83" t="n">
         <v>31</v>
       </c>
-      <c r="F83" s="9" t="n">
+      <c r="F83" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3169,7 +2761,7 @@
       <c r="E84" t="n">
         <v>31</v>
       </c>
-      <c r="F84" s="9" t="n">
+      <c r="F84" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3195,7 +2787,7 @@
       <c r="E85" t="n">
         <v>30</v>
       </c>
-      <c r="F85" s="9" t="n">
+      <c r="F85" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3221,7 +2813,7 @@
       <c r="E86" t="n">
         <v>31</v>
       </c>
-      <c r="F86" s="9" t="n">
+      <c r="F86" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3247,7 +2839,7 @@
       <c r="E87" t="n">
         <v>31</v>
       </c>
-      <c r="F87" s="9" t="n">
+      <c r="F87" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3273,7 +2865,7 @@
       <c r="E88" t="n">
         <v>31</v>
       </c>
-      <c r="F88" s="9" t="n">
+      <c r="F88" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3299,7 +2891,7 @@
       <c r="E89" t="n">
         <v>30</v>
       </c>
-      <c r="F89" s="9" t="n">
+      <c r="F89" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3325,7 +2917,7 @@
       <c r="E90" t="n">
         <v>31</v>
       </c>
-      <c r="F90" s="9" t="n">
+      <c r="F90" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3351,7 +2943,7 @@
       <c r="E91" t="n">
         <v>31</v>
       </c>
-      <c r="F91" s="9" t="n">
+      <c r="F91" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3377,7 +2969,7 @@
       <c r="E92" t="n">
         <v>31</v>
       </c>
-      <c r="F92" s="9" t="n">
+      <c r="F92" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3403,7 +2995,7 @@
       <c r="E93" t="n">
         <v>30</v>
       </c>
-      <c r="F93" s="9" t="n">
+      <c r="F93" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3429,7 +3021,7 @@
       <c r="E94" t="n">
         <v>31</v>
       </c>
-      <c r="F94" s="9" t="n">
+      <c r="F94" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3455,7 +3047,7 @@
       <c r="E95" t="n">
         <v>31</v>
       </c>
-      <c r="F95" s="9" t="n">
+      <c r="F95" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3481,7 +3073,7 @@
       <c r="E96" t="n">
         <v>31</v>
       </c>
-      <c r="F96" s="9" t="n">
+      <c r="F96" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3507,7 +3099,7 @@
       <c r="E97" t="n">
         <v>30</v>
       </c>
-      <c r="F97" s="9" t="n">
+      <c r="F97" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3533,7 +3125,7 @@
       <c r="E98" t="n">
         <v>31</v>
       </c>
-      <c r="F98" s="9" t="n">
+      <c r="F98" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3559,7 +3151,7 @@
       <c r="E99" t="n">
         <v>31</v>
       </c>
-      <c r="F99" s="9" t="n">
+      <c r="F99" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3585,7 +3177,7 @@
       <c r="E100" t="n">
         <v>31</v>
       </c>
-      <c r="F100" s="9" t="n">
+      <c r="F100" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3611,7 +3203,7 @@
       <c r="E101" t="n">
         <v>31</v>
       </c>
-      <c r="F101" s="9" t="n">
+      <c r="F101" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3637,7 +3229,7 @@
       <c r="E102" t="n">
         <v>30</v>
       </c>
-      <c r="F102" s="9" t="n">
+      <c r="F102" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3663,7 +3255,7 @@
       <c r="E103" t="n">
         <v>30</v>
       </c>
-      <c r="F103" s="9" t="n">
+      <c r="F103" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3689,7 +3281,7 @@
       <c r="E104" t="n">
         <v>31</v>
       </c>
-      <c r="F104" s="9" t="n">
+      <c r="F104" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3715,7 +3307,7 @@
       <c r="E105" t="n">
         <v>31</v>
       </c>
-      <c r="F105" s="9" t="n">
+      <c r="F105" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3741,7 +3333,7 @@
       <c r="E106" t="n">
         <v>31</v>
       </c>
-      <c r="F106" s="9" t="n">
+      <c r="F106" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3767,7 +3359,7 @@
       <c r="E107" t="n">
         <v>31</v>
       </c>
-      <c r="F107" s="9" t="n">
+      <c r="F107" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3793,7 +3385,7 @@
       <c r="E108" t="n">
         <v>31</v>
       </c>
-      <c r="F108" s="9" t="n">
+      <c r="F108" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3819,7 +3411,7 @@
       <c r="E109" t="n">
         <v>31</v>
       </c>
-      <c r="F109" s="9" t="n">
+      <c r="F109" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -3845,7 +3437,7 @@
       <c r="E110" t="n">
         <v>30</v>
       </c>
-      <c r="F110" s="9" t="n">
+      <c r="F110" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3871,7 +3463,7 @@
       <c r="E111" t="n">
         <v>30</v>
       </c>
-      <c r="F111" s="9" t="n">
+      <c r="F111" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -3897,7 +3489,7 @@
       <c r="E112" t="n">
         <v>31</v>
       </c>
-      <c r="F112" s="9" t="n">
+      <c r="F112" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3923,7 +3515,7 @@
       <c r="E113" t="n">
         <v>31</v>
       </c>
-      <c r="F113" s="9" t="n">
+      <c r="F113" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -3949,7 +3541,7 @@
       <c r="E114" t="n">
         <v>31</v>
       </c>
-      <c r="F114" s="9" t="n">
+      <c r="F114" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -3975,7 +3567,7 @@
       <c r="E115" t="n">
         <v>31</v>
       </c>
-      <c r="F115" s="9" t="n">
+      <c r="F115" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -4001,7 +3593,7 @@
       <c r="E116" t="n">
         <v>31</v>
       </c>
-      <c r="F116" s="9" t="n">
+      <c r="F116" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4027,7 +3619,7 @@
       <c r="E117" t="n">
         <v>31</v>
       </c>
-      <c r="F117" s="9" t="n">
+      <c r="F117" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4053,7 +3645,7 @@
       <c r="E118" t="n">
         <v>30</v>
       </c>
-      <c r="F118" s="9" t="n">
+      <c r="F118" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -4079,7 +3671,7 @@
       <c r="E119" t="n">
         <v>30</v>
       </c>
-      <c r="F119" s="9" t="n">
+      <c r="F119" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -4105,7 +3697,7 @@
       <c r="E120" t="n">
         <v>31</v>
       </c>
-      <c r="F120" s="9" t="n">
+      <c r="F120" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -4131,7 +3723,7 @@
       <c r="E121" t="n">
         <v>31</v>
       </c>
-      <c r="F121" s="9" t="n">
+      <c r="F121" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -4157,7 +3749,7 @@
       <c r="E122" t="n">
         <v>31</v>
       </c>
-      <c r="F122" s="9" t="n">
+      <c r="F122" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -4183,7 +3775,7 @@
       <c r="E123" t="n">
         <v>31</v>
       </c>
-      <c r="F123" s="9" t="n">
+      <c r="F123" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -4209,7 +3801,7 @@
       <c r="E124" t="n">
         <v>31</v>
       </c>
-      <c r="F124" s="9" t="n">
+      <c r="F124" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4235,7 +3827,7 @@
       <c r="E125" t="n">
         <v>31</v>
       </c>
-      <c r="F125" s="9" t="n">
+      <c r="F125" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4261,7 +3853,7 @@
       <c r="E126" t="n">
         <v>30</v>
       </c>
-      <c r="F126" s="9" t="n">
+      <c r="F126" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -4287,7 +3879,7 @@
       <c r="E127" t="n">
         <v>30</v>
       </c>
-      <c r="F127" s="9" t="n">
+      <c r="F127" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -4313,7 +3905,7 @@
       <c r="E128" t="n">
         <v>31</v>
       </c>
-      <c r="F128" s="9" t="n">
+      <c r="F128" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -4339,7 +3931,7 @@
       <c r="E129" t="n">
         <v>31</v>
       </c>
-      <c r="F129" s="9" t="n">
+      <c r="F129" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -4365,7 +3957,7 @@
       <c r="E130" t="n">
         <v>31</v>
       </c>
-      <c r="F130" s="9" t="n">
+      <c r="F130" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -4391,7 +3983,7 @@
       <c r="E131" t="n">
         <v>31</v>
       </c>
-      <c r="F131" s="9" t="n">
+      <c r="F131" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -4417,7 +4009,7 @@
       <c r="E132" t="n">
         <v>31</v>
       </c>
-      <c r="F132" s="9" t="n">
+      <c r="F132" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4443,7 +4035,7 @@
       <c r="E133" t="n">
         <v>30</v>
       </c>
-      <c r="F133" s="9" t="n">
+      <c r="F133" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -4469,7 +4061,7 @@
       <c r="E134" t="n">
         <v>31</v>
       </c>
-      <c r="F134" s="9" t="n">
+      <c r="F134" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -4495,7 +4087,7 @@
       <c r="E135" t="n">
         <v>31</v>
       </c>
-      <c r="F135" s="9" t="n">
+      <c r="F135" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -4521,7 +4113,7 @@
       <c r="E136" t="n">
         <v>31</v>
       </c>
-      <c r="F136" s="9" t="n">
+      <c r="F136" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4547,7 +4139,7 @@
       <c r="E137" t="n">
         <v>30</v>
       </c>
-      <c r="F137" s="9" t="n">
+      <c r="F137" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -4573,7 +4165,7 @@
       <c r="E138" t="n">
         <v>31</v>
       </c>
-      <c r="F138" s="9" t="n">
+      <c r="F138" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -4599,7 +4191,7 @@
       <c r="E139" t="n">
         <v>31</v>
       </c>
-      <c r="F139" s="9" t="n">
+      <c r="F139" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -4625,7 +4217,7 @@
       <c r="E140" t="n">
         <v>31</v>
       </c>
-      <c r="F140" s="9" t="n">
+      <c r="F140" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4651,7 +4243,7 @@
       <c r="E141" t="n">
         <v>30</v>
       </c>
-      <c r="F141" s="9" t="n">
+      <c r="F141" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -4677,7 +4269,7 @@
       <c r="E142" t="n">
         <v>31</v>
       </c>
-      <c r="F142" s="9" t="n">
+      <c r="F142" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -4703,7 +4295,7 @@
       <c r="E143" t="n">
         <v>31</v>
       </c>
-      <c r="F143" s="9" t="n">
+      <c r="F143" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -4729,7 +4321,7 @@
       <c r="E144" t="n">
         <v>31</v>
       </c>
-      <c r="F144" s="9" t="n">
+      <c r="F144" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4755,7 +4347,7 @@
       <c r="E145" t="n">
         <v>30</v>
       </c>
-      <c r="F145" s="9" t="n">
+      <c r="F145" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -4781,7 +4373,7 @@
       <c r="E146" t="n">
         <v>31</v>
       </c>
-      <c r="F146" s="9" t="n">
+      <c r="F146" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -4807,7 +4399,7 @@
       <c r="E147" t="n">
         <v>31</v>
       </c>
-      <c r="F147" s="9" t="n">
+      <c r="F147" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -4833,7 +4425,7 @@
       <c r="E148" t="n">
         <v>31</v>
       </c>
-      <c r="F148" s="9" t="n">
+      <c r="F148" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4859,7 +4451,7 @@
       <c r="E149" t="n">
         <v>31</v>
       </c>
-      <c r="F149" s="9" t="n">
+      <c r="F149" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4885,7 +4477,7 @@
       <c r="E150" t="n">
         <v>31</v>
       </c>
-      <c r="F150" s="9" t="n">
+      <c r="F150" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4911,7 +4503,7 @@
       <c r="E151" t="n">
         <v>31</v>
       </c>
-      <c r="F151" s="9" t="n">
+      <c r="F151" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -4937,7 +4529,7 @@
       <c r="E152" t="n">
         <v>30</v>
       </c>
-      <c r="F152" s="9" t="n">
+      <c r="F152" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -4963,7 +4555,7 @@
       <c r="E153" t="n">
         <v>31</v>
       </c>
-      <c r="F153" s="9" t="n">
+      <c r="F153" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -4989,7 +4581,7 @@
       <c r="E154" t="n">
         <v>31</v>
       </c>
-      <c r="F154" s="9" t="n">
+      <c r="F154" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5015,7 +4607,7 @@
       <c r="E155" t="n">
         <v>31</v>
       </c>
-      <c r="F155" s="9" t="n">
+      <c r="F155" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5041,7 +4633,7 @@
       <c r="E156" t="n">
         <v>30</v>
       </c>
-      <c r="F156" s="9" t="n">
+      <c r="F156" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -5067,7 +4659,7 @@
       <c r="E157" t="n">
         <v>31</v>
       </c>
-      <c r="F157" s="9" t="n">
+      <c r="F157" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -5093,7 +4685,7 @@
       <c r="E158" t="n">
         <v>31</v>
       </c>
-      <c r="F158" s="9" t="n">
+      <c r="F158" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5119,7 +4711,7 @@
       <c r="E159" t="n">
         <v>31</v>
       </c>
-      <c r="F159" s="9" t="n">
+      <c r="F159" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5145,7 +4737,7 @@
       <c r="E160" t="n">
         <v>31</v>
       </c>
-      <c r="F160" s="9" t="n">
+      <c r="F160" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5171,7 +4763,7 @@
       <c r="E161" t="n">
         <v>30</v>
       </c>
-      <c r="F161" s="9" t="n">
+      <c r="F161" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -5197,7 +4789,7 @@
       <c r="E162" t="n">
         <v>31</v>
       </c>
-      <c r="F162" s="9" t="n">
+      <c r="F162" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -5223,7 +4815,7 @@
       <c r="E163" t="n">
         <v>31</v>
       </c>
-      <c r="F163" s="9" t="n">
+      <c r="F163" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5249,7 +4841,7 @@
       <c r="E164" t="n">
         <v>31</v>
       </c>
-      <c r="F164" s="9" t="n">
+      <c r="F164" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5275,7 +4867,7 @@
       <c r="E165" t="n">
         <v>30</v>
       </c>
-      <c r="F165" s="9" t="n">
+      <c r="F165" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -5301,7 +4893,7 @@
       <c r="E166" t="n">
         <v>31</v>
       </c>
-      <c r="F166" s="9" t="n">
+      <c r="F166" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -5327,7 +4919,7 @@
       <c r="E167" t="n">
         <v>31</v>
       </c>
-      <c r="F167" s="9" t="n">
+      <c r="F167" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5353,7 +4945,7 @@
       <c r="E168" t="n">
         <v>31</v>
       </c>
-      <c r="F168" s="9" t="n">
+      <c r="F168" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5379,7 +4971,7 @@
       <c r="E169" t="n">
         <v>31</v>
       </c>
-      <c r="F169" s="9" t="n">
+      <c r="F169" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5405,7 +4997,7 @@
       <c r="E170" t="n">
         <v>31</v>
       </c>
-      <c r="F170" s="9" t="n">
+      <c r="F170" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5431,7 +5023,7 @@
       <c r="E171" t="n">
         <v>30</v>
       </c>
-      <c r="F171" s="9" t="n">
+      <c r="F171" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -5457,7 +5049,7 @@
       <c r="E172" t="n">
         <v>31</v>
       </c>
-      <c r="F172" s="9" t="n">
+      <c r="F172" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -5483,7 +5075,7 @@
       <c r="E173" t="n">
         <v>31</v>
       </c>
-      <c r="F173" s="9" t="n">
+      <c r="F173" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5509,7 +5101,7 @@
       <c r="E174" t="n">
         <v>31</v>
       </c>
-      <c r="F174" s="9" t="n">
+      <c r="F174" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5535,7 +5127,7 @@
       <c r="E175" t="n">
         <v>30</v>
       </c>
-      <c r="F175" s="9" t="n">
+      <c r="F175" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -5561,7 +5153,7 @@
       <c r="E176" t="n">
         <v>31</v>
       </c>
-      <c r="F176" s="9" t="n">
+      <c r="F176" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -5587,7 +5179,7 @@
       <c r="E177" t="n">
         <v>31</v>
       </c>
-      <c r="F177" s="9" t="n">
+      <c r="F177" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5613,7 +5205,7 @@
       <c r="E178" t="n">
         <v>31</v>
       </c>
-      <c r="F178" s="9" t="n">
+      <c r="F178" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5639,7 +5231,7 @@
       <c r="E179" t="n">
         <v>30</v>
       </c>
-      <c r="F179" s="9" t="n">
+      <c r="F179" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -5665,7 +5257,7 @@
       <c r="E180" t="n">
         <v>31</v>
       </c>
-      <c r="F180" s="9" t="n">
+      <c r="F180" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -5691,7 +5283,7 @@
       <c r="E181" t="n">
         <v>31</v>
       </c>
-      <c r="F181" s="9" t="n">
+      <c r="F181" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5717,7 +5309,7 @@
       <c r="E182" t="n">
         <v>31</v>
       </c>
-      <c r="F182" s="9" t="n">
+      <c r="F182" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5743,7 +5335,7 @@
       <c r="E183" t="n">
         <v>31</v>
       </c>
-      <c r="F183" s="9" t="n">
+      <c r="F183" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5769,7 +5361,7 @@
       <c r="E184" t="n">
         <v>31</v>
       </c>
-      <c r="F184" s="9" t="n">
+      <c r="F184" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5795,7 +5387,7 @@
       <c r="E185" t="n">
         <v>30</v>
       </c>
-      <c r="F185" s="9" t="n">
+      <c r="F185" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -5821,7 +5413,7 @@
       <c r="E186" t="n">
         <v>31</v>
       </c>
-      <c r="F186" s="9" t="n">
+      <c r="F186" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -5847,7 +5439,7 @@
       <c r="E187" t="n">
         <v>31</v>
       </c>
-      <c r="F187" s="9" t="n">
+      <c r="F187" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5873,7 +5465,7 @@
       <c r="E188" t="n">
         <v>31</v>
       </c>
-      <c r="F188" s="9" t="n">
+      <c r="F188" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -5899,7 +5491,7 @@
       <c r="E189" t="n">
         <v>30</v>
       </c>
-      <c r="F189" s="9" t="n">
+      <c r="F189" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -5925,7 +5517,7 @@
       <c r="E190" t="n">
         <v>31</v>
       </c>
-      <c r="F190" s="9" t="n">
+      <c r="F190" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -5951,7 +5543,7 @@
       <c r="E191" t="n">
         <v>31</v>
       </c>
-      <c r="F191" s="9" t="n">
+      <c r="F191" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -5977,7 +5569,7 @@
       <c r="E192" t="n">
         <v>31</v>
       </c>
-      <c r="F192" s="9" t="n">
+      <c r="F192" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6003,7 +5595,7 @@
       <c r="E193" t="n">
         <v>30</v>
       </c>
-      <c r="F193" s="9" t="n">
+      <c r="F193" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -6029,7 +5621,7 @@
       <c r="E194" t="n">
         <v>31</v>
       </c>
-      <c r="F194" s="9" t="n">
+      <c r="F194" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -6055,7 +5647,7 @@
       <c r="E195" t="n">
         <v>31</v>
       </c>
-      <c r="F195" s="9" t="n">
+      <c r="F195" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6081,7 +5673,7 @@
       <c r="E196" t="n">
         <v>31</v>
       </c>
-      <c r="F196" s="9" t="n">
+      <c r="F196" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6107,7 +5699,7 @@
       <c r="E197" t="n">
         <v>31</v>
       </c>
-      <c r="F197" s="9" t="n">
+      <c r="F197" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6133,7 +5725,7 @@
       <c r="E198" t="n">
         <v>31</v>
       </c>
-      <c r="F198" s="9" t="n">
+      <c r="F198" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6159,7 +5751,7 @@
       <c r="E199" t="n">
         <v>30</v>
       </c>
-      <c r="F199" s="9" t="n">
+      <c r="F199" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -6185,7 +5777,7 @@
       <c r="E200" t="n">
         <v>31</v>
       </c>
-      <c r="F200" s="9" t="n">
+      <c r="F200" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -6211,7 +5803,7 @@
       <c r="E201" t="n">
         <v>31</v>
       </c>
-      <c r="F201" s="9" t="n">
+      <c r="F201" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6237,7 +5829,7 @@
       <c r="E202" t="n">
         <v>31</v>
       </c>
-      <c r="F202" s="9" t="n">
+      <c r="F202" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6263,7 +5855,7 @@
       <c r="E203" t="n">
         <v>31</v>
       </c>
-      <c r="F203" s="9" t="n">
+      <c r="F203" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6289,7 +5881,7 @@
       <c r="E204" t="n">
         <v>31</v>
       </c>
-      <c r="F204" s="9" t="n">
+      <c r="F204" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6315,7 +5907,7 @@
       <c r="E205" t="n">
         <v>31</v>
       </c>
-      <c r="F205" s="9" t="n">
+      <c r="F205" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6341,7 +5933,7 @@
       <c r="E206" t="n">
         <v>31</v>
       </c>
-      <c r="F206" s="9" t="n">
+      <c r="F206" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6367,7 +5959,7 @@
       <c r="E207" t="n">
         <v>30</v>
       </c>
-      <c r="F207" s="9" t="n">
+      <c r="F207" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -6393,7 +5985,7 @@
       <c r="E208" t="n">
         <v>31</v>
       </c>
-      <c r="F208" s="9" t="n">
+      <c r="F208" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -6419,7 +6011,7 @@
       <c r="E209" t="n">
         <v>31</v>
       </c>
-      <c r="F209" s="9" t="n">
+      <c r="F209" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6445,7 +6037,7 @@
       <c r="E210" t="n">
         <v>31</v>
       </c>
-      <c r="F210" s="9" t="n">
+      <c r="F210" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6471,7 +6063,7 @@
       <c r="E211" t="n">
         <v>31</v>
       </c>
-      <c r="F211" s="9" t="n">
+      <c r="F211" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6497,7 +6089,7 @@
       <c r="E212" t="n">
         <v>31</v>
       </c>
-      <c r="F212" s="9" t="n">
+      <c r="F212" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6523,7 +6115,7 @@
       <c r="E213" t="n">
         <v>31</v>
       </c>
-      <c r="F213" s="9" t="n">
+      <c r="F213" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6549,7 +6141,7 @@
       <c r="E214" t="n">
         <v>31</v>
       </c>
-      <c r="F214" s="9" t="n">
+      <c r="F214" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6575,7 +6167,7 @@
       <c r="E215" t="n">
         <v>30</v>
       </c>
-      <c r="F215" s="9" t="n">
+      <c r="F215" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -6601,7 +6193,7 @@
       <c r="E216" t="n">
         <v>31</v>
       </c>
-      <c r="F216" s="9" t="n">
+      <c r="F216" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -6627,7 +6219,7 @@
       <c r="E217" t="n">
         <v>31</v>
       </c>
-      <c r="F217" s="9" t="n">
+      <c r="F217" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6653,7 +6245,7 @@
       <c r="E218" t="n">
         <v>31</v>
       </c>
-      <c r="F218" s="9" t="n">
+      <c r="F218" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6679,7 +6271,7 @@
       <c r="E219" t="n">
         <v>30</v>
       </c>
-      <c r="F219" s="9" t="n">
+      <c r="F219" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -6705,7 +6297,7 @@
       <c r="E220" t="n">
         <v>31</v>
       </c>
-      <c r="F220" s="9" t="n">
+      <c r="F220" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -6731,7 +6323,7 @@
       <c r="E221" t="n">
         <v>31</v>
       </c>
-      <c r="F221" s="9" t="n">
+      <c r="F221" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6757,7 +6349,7 @@
       <c r="E222" t="n">
         <v>31</v>
       </c>
-      <c r="F222" s="9" t="n">
+      <c r="F222" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6783,7 +6375,7 @@
       <c r="E223" t="n">
         <v>30</v>
       </c>
-      <c r="F223" s="9" t="n">
+      <c r="F223" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -6809,7 +6401,7 @@
       <c r="E224" t="n">
         <v>31</v>
       </c>
-      <c r="F224" s="9" t="n">
+      <c r="F224" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -6835,7 +6427,7 @@
       <c r="E225" t="n">
         <v>31</v>
       </c>
-      <c r="F225" s="9" t="n">
+      <c r="F225" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6861,7 +6453,7 @@
       <c r="E226" t="n">
         <v>31</v>
       </c>
-      <c r="F226" s="9" t="n">
+      <c r="F226" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6887,7 +6479,7 @@
       <c r="E227" t="n">
         <v>30</v>
       </c>
-      <c r="F227" s="9" t="n">
+      <c r="F227" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -6913,7 +6505,7 @@
       <c r="E228" t="n">
         <v>31</v>
       </c>
-      <c r="F228" s="9" t="n">
+      <c r="F228" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -6939,7 +6531,7 @@
       <c r="E229" t="n">
         <v>31</v>
       </c>
-      <c r="F229" s="9" t="n">
+      <c r="F229" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -6965,7 +6557,7 @@
       <c r="E230" t="n">
         <v>31</v>
       </c>
-      <c r="F230" s="9" t="n">
+      <c r="F230" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -6991,7 +6583,7 @@
       <c r="E231" t="n">
         <v>30</v>
       </c>
-      <c r="F231" s="9" t="n">
+      <c r="F231" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7017,7 +6609,7 @@
       <c r="E232" t="n">
         <v>31</v>
       </c>
-      <c r="F232" s="9" t="n">
+      <c r="F232" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7043,7 +6635,7 @@
       <c r="E233" t="n">
         <v>31</v>
       </c>
-      <c r="F233" s="9" t="n">
+      <c r="F233" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -7069,7 +6661,7 @@
       <c r="E234" t="n">
         <v>31</v>
       </c>
-      <c r="F234" s="9" t="n">
+      <c r="F234" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -7095,7 +6687,7 @@
       <c r="E235" t="n">
         <v>30</v>
       </c>
-      <c r="F235" s="9" t="n">
+      <c r="F235" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7121,7 +6713,7 @@
       <c r="E236" t="n">
         <v>31</v>
       </c>
-      <c r="F236" s="9" t="n">
+      <c r="F236" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7147,7 +6739,7 @@
       <c r="E237" t="n">
         <v>31</v>
       </c>
-      <c r="F237" s="9" t="n">
+      <c r="F237" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -7173,7 +6765,7 @@
       <c r="E238" t="n">
         <v>31</v>
       </c>
-      <c r="F238" s="9" t="n">
+      <c r="F238" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -7199,7 +6791,7 @@
       <c r="E239" t="n">
         <v>30</v>
       </c>
-      <c r="F239" s="9" t="n">
+      <c r="F239" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7225,7 +6817,7 @@
       <c r="E240" t="n">
         <v>31</v>
       </c>
-      <c r="F240" s="9" t="n">
+      <c r="F240" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7251,7 +6843,7 @@
       <c r="E241" t="n">
         <v>31</v>
       </c>
-      <c r="F241" s="9" t="n">
+      <c r="F241" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -7277,7 +6869,7 @@
       <c r="E242" t="n">
         <v>31</v>
       </c>
-      <c r="F242" s="9" t="n">
+      <c r="F242" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -7303,7 +6895,7 @@
       <c r="E243" t="n">
         <v>30</v>
       </c>
-      <c r="F243" s="9" t="n">
+      <c r="F243" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7329,7 +6921,7 @@
       <c r="E244" t="n">
         <v>31</v>
       </c>
-      <c r="F244" s="9" t="n">
+      <c r="F244" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7355,7 +6947,7 @@
       <c r="E245" t="n">
         <v>31</v>
       </c>
-      <c r="F245" s="9" t="n">
+      <c r="F245" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -7381,7 +6973,7 @@
       <c r="E246" t="n">
         <v>31</v>
       </c>
-      <c r="F246" s="9" t="n">
+      <c r="F246" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -7407,7 +6999,7 @@
       <c r="E247" t="n">
         <v>30</v>
       </c>
-      <c r="F247" s="9" t="n">
+      <c r="F247" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7433,7 +7025,7 @@
       <c r="E248" t="n">
         <v>31</v>
       </c>
-      <c r="F248" s="9" t="n">
+      <c r="F248" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7459,7 +7051,7 @@
       <c r="E249" t="n">
         <v>31</v>
       </c>
-      <c r="F249" s="9" t="n">
+      <c r="F249" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -7485,7 +7077,7 @@
       <c r="E250" t="n">
         <v>31</v>
       </c>
-      <c r="F250" s="9" t="n">
+      <c r="F250" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -7511,7 +7103,7 @@
       <c r="E251" t="n">
         <v>30</v>
       </c>
-      <c r="F251" s="9" t="n">
+      <c r="F251" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7537,7 +7129,7 @@
       <c r="E252" t="n">
         <v>31</v>
       </c>
-      <c r="F252" s="9" t="n">
+      <c r="F252" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7563,7 +7155,7 @@
       <c r="E253" t="n">
         <v>31</v>
       </c>
-      <c r="F253" s="9" t="n">
+      <c r="F253" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -7589,7 +7181,7 @@
       <c r="E254" t="n">
         <v>31</v>
       </c>
-      <c r="F254" s="9" t="n">
+      <c r="F254" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -7615,7 +7207,7 @@
       <c r="E255" t="n">
         <v>30</v>
       </c>
-      <c r="F255" s="9" t="n">
+      <c r="F255" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7641,7 +7233,7 @@
       <c r="E256" t="n">
         <v>31</v>
       </c>
-      <c r="F256" s="9" t="n">
+      <c r="F256" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7667,7 +7259,7 @@
       <c r="E257" t="n">
         <v>31</v>
       </c>
-      <c r="F257" s="9" t="n">
+      <c r="F257" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -7693,7 +7285,7 @@
       <c r="E258" t="n">
         <v>31</v>
       </c>
-      <c r="F258" s="9" t="n">
+      <c r="F258" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -7719,7 +7311,7 @@
       <c r="E259" t="n">
         <v>30</v>
       </c>
-      <c r="F259" s="9" t="n">
+      <c r="F259" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7745,7 +7337,7 @@
       <c r="E260" t="n">
         <v>31</v>
       </c>
-      <c r="F260" s="9" t="n">
+      <c r="F260" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7771,7 +7363,7 @@
       <c r="E261" t="n">
         <v>31</v>
       </c>
-      <c r="F261" s="9" t="n">
+      <c r="F261" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -7797,7 +7389,7 @@
       <c r="E262" t="n">
         <v>31</v>
       </c>
-      <c r="F262" s="9" t="n">
+      <c r="F262" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -7823,7 +7415,7 @@
       <c r="E263" t="n">
         <v>30</v>
       </c>
-      <c r="F263" s="9" t="n">
+      <c r="F263" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7849,7 +7441,7 @@
       <c r="E264" t="n">
         <v>31</v>
       </c>
-      <c r="F264" s="9" t="n">
+      <c r="F264" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7875,7 +7467,7 @@
       <c r="E265" t="n">
         <v>31</v>
       </c>
-      <c r="F265" s="9" t="n">
+      <c r="F265" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -7901,7 +7493,7 @@
       <c r="E266" t="n">
         <v>31</v>
       </c>
-      <c r="F266" s="9" t="n">
+      <c r="F266" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -7927,7 +7519,7 @@
       <c r="E267" t="n">
         <v>30</v>
       </c>
-      <c r="F267" s="9" t="n">
+      <c r="F267" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -7953,7 +7545,7 @@
       <c r="E268" t="n">
         <v>31</v>
       </c>
-      <c r="F268" s="9" t="n">
+      <c r="F268" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -7979,7 +7571,7 @@
       <c r="E269" t="n">
         <v>31</v>
       </c>
-      <c r="F269" s="9" t="n">
+      <c r="F269" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -8005,7 +7597,7 @@
       <c r="E270" t="n">
         <v>31</v>
       </c>
-      <c r="F270" s="9" t="n">
+      <c r="F270" s="8" t="n">
         <v>45682.54166666666</v>
       </c>
     </row>
@@ -8031,7 +7623,7 @@
       <c r="E271" t="n">
         <v>30</v>
       </c>
-      <c r="F271" s="9" t="n">
+      <c r="F271" s="8" t="n">
         <v>46047.375</v>
       </c>
     </row>
@@ -8057,7 +7649,7 @@
       <c r="E272" t="n">
         <v>31</v>
       </c>
-      <c r="F272" s="9" t="n">
+      <c r="F272" s="8" t="n">
         <v>46047.41666666666</v>
       </c>
     </row>
@@ -8083,7 +7675,319 @@
       <c r="E273" t="n">
         <v>31</v>
       </c>
-      <c r="F273" s="9" t="n">
+      <c r="F273" s="8" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>100</v>
+      </c>
+      <c r="E274" t="n">
+        <v>31</v>
+      </c>
+      <c r="F274" s="8" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>1</v>
+      </c>
+      <c r="E275" t="n">
+        <v>30</v>
+      </c>
+      <c r="F275" s="8" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>1</v>
+      </c>
+      <c r="E276" t="n">
+        <v>31</v>
+      </c>
+      <c r="F276" s="8" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>1</v>
+      </c>
+      <c r="E277" t="n">
+        <v>31</v>
+      </c>
+      <c r="F277" s="8" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>100</v>
+      </c>
+      <c r="E278" t="n">
+        <v>31</v>
+      </c>
+      <c r="F278" s="8" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>1</v>
+      </c>
+      <c r="E279" t="n">
+        <v>30</v>
+      </c>
+      <c r="F279" s="8" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>1</v>
+      </c>
+      <c r="E280" t="n">
+        <v>31</v>
+      </c>
+      <c r="F280" s="8" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>1</v>
+      </c>
+      <c r="E281" t="n">
+        <v>31</v>
+      </c>
+      <c r="F281" s="8" t="n">
+        <v>46047.54166666666</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>100</v>
+      </c>
+      <c r="E282" t="n">
+        <v>31</v>
+      </c>
+      <c r="F282" s="8" t="n">
+        <v>45682.54166666666</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Compra A</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>1</v>
+      </c>
+      <c r="E283" t="n">
+        <v>30</v>
+      </c>
+      <c r="F283" s="8" t="n">
+        <v>46047.375</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Compra B</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>1</v>
+      </c>
+      <c r="E284" t="n">
+        <v>31</v>
+      </c>
+      <c r="F284" s="8" t="n">
+        <v>46047.41666666666</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAM VERM POLO </t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>1</v>
+      </c>
+      <c r="E285" t="n">
+        <v>31</v>
+      </c>
+      <c r="F285" s="8" t="n">
         <v>46047.54166666666</v>
       </c>
     </row>
@@ -8597,7 +8501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8606,34 +8510,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Nome do produto</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Tipo</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Tamanho</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Valor unitario</t>
-        </is>
-      </c>
-      <c r="F1" s="7" t="inlineStr">
-        <is>
-          <t>Valor unitario compra</t>
         </is>
       </c>
     </row>
@@ -8659,7 +8558,6 @@
       <c r="E2" t="n">
         <v>30</v>
       </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8683,7 +8581,6 @@
       <c r="E3" t="n">
         <v>31</v>
       </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8707,7 +8604,6 @@
       <c r="E4" t="n">
         <v>31</v>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8731,7 +8627,6 @@
       <c r="E5" t="n">
         <v>31</v>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8750,12 +8645,11 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>7051</v>
+        <v>7348</v>
       </c>
       <c r="E6" t="n">
         <v>31</v>
       </c>
-      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -8763,18 +8657,13 @@
           <t>Compra A</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>16</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -8783,18 +8672,13 @@
           <t>Compra A</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>16</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -8803,18 +8687,13 @@
           <t>Compra B</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>16</v>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>